<commit_message>
added new bgm data for deliveries
</commit_message>
<xml_diff>
--- a/data/custom_time_distribution_vacc.xlsx
+++ b/data/custom_time_distribution_vacc.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects_personal\vaccination_dashboard\impftracker\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EEC23E4-37A2-4C69-B8D1-89513CEABB83}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F67178E-54D7-4F88-AD30-4C53490C7F2F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="template" sheetId="1" r:id="rId1"/>
     <sheet name="custom_jj" sheetId="2" r:id="rId2"/>
+    <sheet name="bgm_data" sheetId="4" r:id="rId3"/>
+    <sheet name="Tabelle1" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="26">
   <si>
     <t>year</t>
   </si>
@@ -62,6 +64,54 @@
   </si>
   <si>
     <t>sanofi</t>
+  </si>
+  <si>
+    <t>KW 14</t>
+  </si>
+  <si>
+    <t>KW 15</t>
+  </si>
+  <si>
+    <t>KW 16</t>
+  </si>
+  <si>
+    <t>KW 17</t>
+  </si>
+  <si>
+    <t>KW 18</t>
+  </si>
+  <si>
+    <t>KW 19</t>
+  </si>
+  <si>
+    <t>KW 20</t>
+  </si>
+  <si>
+    <t>KW 21</t>
+  </si>
+  <si>
+    <t>KW 22</t>
+  </si>
+  <si>
+    <t>KW 23</t>
+  </si>
+  <si>
+    <t>KW 24</t>
+  </si>
+  <si>
+    <t>KW 25</t>
+  </si>
+  <si>
+    <t>KW 26</t>
+  </si>
+  <si>
+    <t>Quartal</t>
+  </si>
+  <si>
+    <t>moderna_aufgeteilt</t>
+  </si>
+  <si>
+    <t>pfizer_aufgeteilt</t>
   </si>
 </sst>
 </file>
@@ -120,12 +170,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1944,7 +1996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27CD4EC4-33C7-448D-9376-C861354FAF0A}">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
@@ -3465,4 +3517,1905 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87642ED8-69AB-4BBC-B131-945791980BF4}">
+  <dimension ref="A1:J55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K17" sqref="K17:K29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2020</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>52</v>
+      </c>
+      <c r="D2" s="2">
+        <v>44186</v>
+      </c>
+      <c r="I2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2020</v>
+      </c>
+      <c r="B3">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>53</v>
+      </c>
+      <c r="D3" s="2">
+        <v>44193</v>
+      </c>
+      <c r="I3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2021</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="2">
+        <v>44200</v>
+      </c>
+      <c r="E4">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H4">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I4">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2021</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2">
+        <v>44207</v>
+      </c>
+      <c r="E5">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H5">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I5">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2021</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44214</v>
+      </c>
+      <c r="E6">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H6">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I6">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2021</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44221</v>
+      </c>
+      <c r="E7">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H7">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I7">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2021</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44228</v>
+      </c>
+      <c r="E8">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H8">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I8">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2021</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>6</v>
+      </c>
+      <c r="D9" s="2">
+        <v>44235</v>
+      </c>
+      <c r="E9">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H9">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I9">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2021</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
+      </c>
+      <c r="D10" s="2">
+        <v>44242</v>
+      </c>
+      <c r="E10">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H10">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I10">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2021</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2">
+        <v>44249</v>
+      </c>
+      <c r="E11">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H11">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I11">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2021</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12" s="2">
+        <v>44256</v>
+      </c>
+      <c r="E12">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H12">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I12">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2">
+        <v>44263</v>
+      </c>
+      <c r="E13">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H13">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I13">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2021</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2">
+        <v>44270</v>
+      </c>
+      <c r="E14">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H14">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I14">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2021</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2">
+        <v>44277</v>
+      </c>
+      <c r="E15">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H15">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I15">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2021</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16" s="2">
+        <v>44284</v>
+      </c>
+      <c r="E16">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H16">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I16">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2021</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>14</v>
+      </c>
+      <c r="D17" s="2">
+        <v>44291</v>
+      </c>
+      <c r="E17">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>8.9906542056074762E-2</v>
+      </c>
+      <c r="I17">
+        <v>5.0005814629608097E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2021</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18">
+        <v>15</v>
+      </c>
+      <c r="D18" s="2">
+        <v>44298</v>
+      </c>
+      <c r="E18">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f>0.26/10.1</f>
+        <v>2.5742574257425745E-2</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>5.0005814629608097E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2021</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2">
+        <v>44305</v>
+      </c>
+      <c r="E19">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>5.1401869158878503E-2</v>
+      </c>
+      <c r="I19">
+        <v>5.0145365740202348E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2021</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20">
+        <v>17</v>
+      </c>
+      <c r="D20" s="2">
+        <v>44312</v>
+      </c>
+      <c r="E20">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <f>0.44/10.1</f>
+        <v>4.3564356435643568E-2</v>
+      </c>
+      <c r="H20">
+        <v>5.8691588785046732E-2</v>
+      </c>
+      <c r="I20">
+        <v>6.8356785672752648E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2021</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21" s="2">
+        <v>44319</v>
+      </c>
+      <c r="E21">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <f>(2.3/4)/10.1</f>
+        <v>5.6930693069306926E-2</v>
+      </c>
+      <c r="H21">
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I21">
+        <v>6.7728805675078496E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2021</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22">
+        <v>19</v>
+      </c>
+      <c r="D22" s="2">
+        <v>44326</v>
+      </c>
+      <c r="E22">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G24" si="0">(2.3/4)/10.1</f>
+        <v>5.6930693069306926E-2</v>
+      </c>
+      <c r="H22">
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I22">
+        <v>6.7728805675078496E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2021</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>20</v>
+      </c>
+      <c r="D23" s="2">
+        <v>44333</v>
+      </c>
+      <c r="E23">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>5.6930693069306926E-2</v>
+      </c>
+      <c r="H23">
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I23">
+        <v>6.7752064193510875E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2021</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>21</v>
+      </c>
+      <c r="D24" s="2">
+        <v>44340</v>
+      </c>
+      <c r="E24">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>5.6930693069306926E-2</v>
+      </c>
+      <c r="H24">
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I24">
+        <v>6.7775322711943253E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2021</v>
+      </c>
+      <c r="B25">
+        <v>2</v>
+      </c>
+      <c r="C25">
+        <v>22</v>
+      </c>
+      <c r="D25" s="2">
+        <v>44347</v>
+      </c>
+      <c r="E25">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <f>(7.1/5)/10.1</f>
+        <v>0.14059405940594058</v>
+      </c>
+      <c r="H25">
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I25">
+        <v>0.10208163739969764</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2021</v>
+      </c>
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>23</v>
+      </c>
+      <c r="D26" s="2">
+        <v>44354</v>
+      </c>
+      <c r="E26">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.25</v>
+      </c>
+      <c r="G26">
+        <f t="shared" ref="G26:G29" si="1">(7.1/5)/10.1</f>
+        <v>0.14059405940594058</v>
+      </c>
+      <c r="H26">
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I26">
+        <v>0.10208163739969764</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2021</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>24</v>
+      </c>
+      <c r="D27" s="2">
+        <v>44361</v>
+      </c>
+      <c r="E27">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F27">
+        <v>0.25</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>0.14059405940594058</v>
+      </c>
+      <c r="H27">
+        <v>9.1214953271028035E-2</v>
+      </c>
+      <c r="I27">
+        <v>0.10208163739969764</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2021</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+      <c r="C28">
+        <v>25</v>
+      </c>
+      <c r="D28" s="2">
+        <v>44368</v>
+      </c>
+      <c r="E28">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F28">
+        <v>0.25</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>0.14059405940594058</v>
+      </c>
+      <c r="H28">
+        <v>9.7009345794392521E-2</v>
+      </c>
+      <c r="I28">
+        <v>0.1021281544365624</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2021</v>
+      </c>
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>26</v>
+      </c>
+      <c r="D29" s="2">
+        <v>44375</v>
+      </c>
+      <c r="E29">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.25</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>0.14059405940594058</v>
+      </c>
+      <c r="H29">
+        <v>9.7009345794392521E-2</v>
+      </c>
+      <c r="I29">
+        <v>0.1021281544365624</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2021</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30">
+        <v>27</v>
+      </c>
+      <c r="D30" s="2">
+        <v>44382</v>
+      </c>
+      <c r="E30">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F30">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G30">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H30">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I30">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2021</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>28</v>
+      </c>
+      <c r="D31" s="2">
+        <v>44389</v>
+      </c>
+      <c r="E31">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F31">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G31">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H31">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I31">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2021</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32">
+        <v>29</v>
+      </c>
+      <c r="D32" s="2">
+        <v>44396</v>
+      </c>
+      <c r="E32">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F32">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G32">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H32">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I32">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2021</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33">
+        <v>30</v>
+      </c>
+      <c r="D33" s="2">
+        <v>44403</v>
+      </c>
+      <c r="E33">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F33">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G33">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H33">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I33">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>2021</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34">
+        <v>31</v>
+      </c>
+      <c r="D34" s="2">
+        <v>44410</v>
+      </c>
+      <c r="E34">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F34">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G34">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H34">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I34">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>2021</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>32</v>
+      </c>
+      <c r="D35" s="2">
+        <v>44417</v>
+      </c>
+      <c r="E35">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F35">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G35">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H35">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I35">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>2021</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36">
+        <v>33</v>
+      </c>
+      <c r="D36" s="2">
+        <v>44424</v>
+      </c>
+      <c r="E36">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F36">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G36">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H36">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I36">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>2021</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37">
+        <v>34</v>
+      </c>
+      <c r="D37" s="2">
+        <v>44431</v>
+      </c>
+      <c r="E37">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F37">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G37">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H37">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I37">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>2021</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38">
+        <v>35</v>
+      </c>
+      <c r="D38" s="2">
+        <v>44438</v>
+      </c>
+      <c r="E38">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F38">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G38">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H38">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I38">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>2021</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39">
+        <v>36</v>
+      </c>
+      <c r="D39" s="2">
+        <v>44445</v>
+      </c>
+      <c r="E39">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F39">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G39">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H39">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I39">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>2021</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40">
+        <v>37</v>
+      </c>
+      <c r="D40" s="2">
+        <v>44452</v>
+      </c>
+      <c r="E40">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F40">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G40">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H40">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I40">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>2021</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41">
+        <v>38</v>
+      </c>
+      <c r="D41" s="2">
+        <v>44459</v>
+      </c>
+      <c r="E41">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F41">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G41">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H41">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I41">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>2021</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42">
+        <v>39</v>
+      </c>
+      <c r="D42" s="2">
+        <v>44466</v>
+      </c>
+      <c r="E42">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="F42">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G42">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H42">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I42">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>2021</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43">
+        <v>40</v>
+      </c>
+      <c r="D43" s="2">
+        <v>44473</v>
+      </c>
+      <c r="F43">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G43">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H43">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I43">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J43">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>2021</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>41</v>
+      </c>
+      <c r="D44" s="2">
+        <v>44480</v>
+      </c>
+      <c r="F44">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G44">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H44">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I44">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J44">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>2021</v>
+      </c>
+      <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45">
+        <v>42</v>
+      </c>
+      <c r="D45" s="2">
+        <v>44487</v>
+      </c>
+      <c r="F45">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G45">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H45">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I45">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J45">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>2021</v>
+      </c>
+      <c r="B46">
+        <v>4</v>
+      </c>
+      <c r="C46">
+        <v>43</v>
+      </c>
+      <c r="D46" s="2">
+        <v>44494</v>
+      </c>
+      <c r="F46">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G46">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H46">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I46">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J46">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <v>2021</v>
+      </c>
+      <c r="B47">
+        <v>4</v>
+      </c>
+      <c r="C47">
+        <v>44</v>
+      </c>
+      <c r="D47" s="2">
+        <v>44501</v>
+      </c>
+      <c r="F47">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G47">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H47">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I47">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J47">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <v>2021</v>
+      </c>
+      <c r="B48">
+        <v>4</v>
+      </c>
+      <c r="C48">
+        <v>45</v>
+      </c>
+      <c r="D48" s="2">
+        <v>44508</v>
+      </c>
+      <c r="F48">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G48">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H48">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I48">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J48">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <v>2021</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>46</v>
+      </c>
+      <c r="D49" s="2">
+        <v>44515</v>
+      </c>
+      <c r="F49">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G49">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H49">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I49">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J49">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <v>2021</v>
+      </c>
+      <c r="B50">
+        <v>4</v>
+      </c>
+      <c r="C50">
+        <v>47</v>
+      </c>
+      <c r="D50" s="2">
+        <v>44522</v>
+      </c>
+      <c r="F50">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G50">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H50">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I50">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J50">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <v>2021</v>
+      </c>
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51">
+        <v>48</v>
+      </c>
+      <c r="D51" s="2">
+        <v>44529</v>
+      </c>
+      <c r="F51">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G51">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H51">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I51">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J51">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <v>2021</v>
+      </c>
+      <c r="B52">
+        <v>4</v>
+      </c>
+      <c r="C52">
+        <v>49</v>
+      </c>
+      <c r="D52" s="2">
+        <v>44536</v>
+      </c>
+      <c r="F52">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G52">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H52">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I52">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J52">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <v>2021</v>
+      </c>
+      <c r="B53">
+        <v>4</v>
+      </c>
+      <c r="C53">
+        <v>50</v>
+      </c>
+      <c r="D53" s="2">
+        <v>44543</v>
+      </c>
+      <c r="F53">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G53">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H53">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I53">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J53">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <v>2021</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>51</v>
+      </c>
+      <c r="D54" s="2">
+        <v>44550</v>
+      </c>
+      <c r="F54">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G54">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H54">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I54">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J54">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <v>2021</v>
+      </c>
+      <c r="B55">
+        <v>4</v>
+      </c>
+      <c r="C55">
+        <v>52</v>
+      </c>
+      <c r="D55" s="2">
+        <v>44557</v>
+      </c>
+      <c r="F55">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="G55">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="H55">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="I55">
+        <v>7.6923076923076927E-2</v>
+      </c>
+      <c r="J55">
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F2D9E7-415F-45C2-B6B1-16DD2B39E66A}">
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="3">
+        <v>577200</v>
+      </c>
+      <c r="C2" s="3">
+        <v>2515500</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2" s="4">
+        <v>44260</v>
+      </c>
+      <c r="H2">
+        <f>B2/SUM(B$2:B$14)</f>
+        <v>8.9906542056074762E-2</v>
+      </c>
+      <c r="I2">
+        <f>C2/SUM(C$2:C$14)</f>
+        <v>5.0005814629608097E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2515500</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4">
+        <v>44298</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H14" si="0">B3/SUM(B$2:B$14)</f>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ref="I3:I14" si="1">C3/SUM(C$2:C$14)</f>
+        <v>5.0005814629608097E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="3">
+        <v>330000</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2522520</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="4">
+        <v>44305</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>5.1401869158878503E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>5.0145365740202348E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="3">
+        <v>376800</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3438630</v>
+      </c>
+      <c r="F5">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4">
+        <v>44312</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>5.8691588785046732E-2</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>6.8356785672752648E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="3">
+        <v>550800</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3407040</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6" s="4">
+        <v>44319</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>6.7728805675078496E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3">
+        <v>550800</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3407040</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+      <c r="G7" s="4">
+        <v>44326</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>6.7728805675078496E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="3">
+        <v>550800</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3408210</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8" s="4">
+        <v>44333</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>6.7752064193510875E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="3">
+        <v>550800</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3409380</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9" s="4">
+        <v>44340</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>6.7775322711943253E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="3">
+        <v>550800</v>
+      </c>
+      <c r="C10" s="3">
+        <v>5135130</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10" s="4">
+        <v>44347</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>0.10208163739969764</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="3">
+        <v>550800</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5135130</v>
+      </c>
+      <c r="F11">
+        <v>2</v>
+      </c>
+      <c r="G11" s="4">
+        <v>44354</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>8.5794392523364488E-2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>0.10208163739969764</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="3">
+        <v>585600</v>
+      </c>
+      <c r="C12" s="3">
+        <v>5135130</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="4">
+        <v>44361</v>
+      </c>
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>9.1214953271028035E-2</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0.10208163739969764</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="3">
+        <v>622800</v>
+      </c>
+      <c r="C13" s="3">
+        <v>5137470</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="4">
+        <v>44368</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>9.7009345794392521E-2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>0.1021281544365624</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" s="3">
+        <v>622800</v>
+      </c>
+      <c r="C14" s="3">
+        <v>5137470</v>
+      </c>
+      <c r="F14">
+        <v>2</v>
+      </c>
+      <c r="G14" s="4">
+        <v>44375</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="0"/>
+        <v>9.7009345794392521E-2</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>0.1021281544365624</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B16">
+        <f>SUM(B2:B14)</f>
+        <v>6420000</v>
+      </c>
+      <c r="C16" s="3">
+        <f>SUM(C2:C14)</f>
+        <v>50304150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>